<commit_message>
Correct D1 inNB3 Hindbrain BOM
</commit_message>
<xml_diff>
--- a/fpgas/NB3_hindbrain/fab/NB3_hindbrain.xlsx
+++ b/fpgas/NB3_hindbrain/fab/NB3_hindbrain.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="157">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -208,19 +208,22 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
+    <t xml:space="preserve">5 mA SMD 0402 White LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yongyu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZYY0402W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C434448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D17,D7,D11,D13,D15,D19,D9,D21,D3</t>
+  </si>
+  <si>
     <t xml:space="preserve">5 mA SMD 0402 Blue LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yongyu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SZYY0402W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C434448</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D17,D7,D11,D13,D15,D19,D9,D21,D3</t>
   </si>
   <si>
     <t xml:space="preserve">SZYY0402B</t>
@@ -497,11 +500,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -521,12 +525,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -593,12 +591,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -606,15 +604,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -698,7 +692,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -749,7 +743,7 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -758,7 +752,7 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -779,7 +773,7 @@
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -809,22 +803,22 @@
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="4" t="n">
         <v>0.0012</v>
       </c>
       <c r="I4" s="1" t="n">
@@ -839,22 +833,22 @@
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="4" t="n">
         <v>0.0009</v>
       </c>
       <c r="I5" s="1" t="n">
@@ -869,10 +863,10 @@
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -899,10 +893,10 @@
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -929,16 +923,16 @@
       <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -959,16 +953,16 @@
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -989,16 +983,16 @@
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1019,10 +1013,10 @@
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1049,16 +1043,16 @@
       <c r="B12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1079,16 +1073,16 @@
       <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1140,19 +1134,19 @@
         <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0.0159</v>
@@ -1167,22 +1161,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0.0139</v>
@@ -1197,22 +1191,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0.3241</v>
@@ -1227,22 +1221,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0.009</v>
@@ -1257,22 +1251,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>0.17</v>
@@ -1287,22 +1281,22 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0.0262</v>
@@ -1317,22 +1311,22 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0.0167</v>
@@ -1347,22 +1341,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0.2135</v>
@@ -1377,22 +1371,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0.4455</v>
@@ -1407,22 +1401,22 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>0.0245</v>
@@ -1437,22 +1431,22 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>0.89</v>
@@ -1467,22 +1461,22 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>0.8448</v>
@@ -1497,22 +1491,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>4.07</v>
@@ -1527,22 +1521,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>7.13</v>
@@ -1557,22 +1551,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>0.2618</v>
@@ -1587,22 +1581,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>2.13</v>
@@ -1617,22 +1611,22 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>2.16</v>
@@ -1647,22 +1641,22 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>0.5298</v>
@@ -1677,22 +1671,22 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>0.091</v>

</xml_diff>